<commit_message>
agregado de notas de electronica y td de 5to
</commit_message>
<xml_diff>
--- a/inasistencias-5a-InstrumentalYsistElect/alumnos-5a-InstrumentalYsistElect.xlsx
+++ b/inasistencias-5a-InstrumentalYsistElect/alumnos-5a-InstrumentalYsistElect.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="asistencia" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="486">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t xml:space="preserve">positivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6+posi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valoracion</t>
   </si>
   <si>
     <t xml:space="preserve">Apellido</t>
@@ -1486,9 +1495,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1562,7 +1572,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1579,6 +1589,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1588,7 +1602,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <b val="1"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="12"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1605,6 +1634,66 @@
       </fill>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1615,7 +1704,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2161,7 +2250,7 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2177,13 +2266,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,10 +2280,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>7</v>
@@ -2208,10 +2297,10 @@
         <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>5</v>
@@ -2233,10 +2322,10 @@
         <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>3</v>
@@ -2247,10 +2336,10 @@
         <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>7</v>
@@ -2261,10 +2350,10 @@
         <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>8</v>
@@ -2286,10 +2375,10 @@
         <v>55</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>7</v>
@@ -2300,10 +2389,10 @@
         <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>6</v>
@@ -2314,10 +2403,10 @@
         <v>55</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>5</v>
@@ -2328,10 +2417,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>5</v>
@@ -2342,10 +2431,10 @@
         <v>55</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>5</v>
@@ -2356,10 +2445,10 @@
         <v>55</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>4</v>
@@ -2370,10 +2459,10 @@
         <v>55</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>3</v>
@@ -2384,10 +2473,10 @@
         <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>3</v>
@@ -2398,10 +2487,10 @@
         <v>61</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>7</v>
@@ -2423,10 +2512,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
@@ -2437,10 +2526,10 @@
         <v>61</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>1</v>
@@ -2451,10 +2540,10 @@
         <v>64</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>7</v>
@@ -2476,10 +2565,10 @@
         <v>64</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>6</v>
@@ -2490,10 +2579,10 @@
         <v>64</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>5</v>
@@ -2504,10 +2593,10 @@
         <v>64</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>5</v>
@@ -2518,10 +2607,10 @@
         <v>64</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>5</v>
@@ -2532,10 +2621,10 @@
         <v>64</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>2</v>
@@ -2559,7 +2648,7 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -2582,22 +2671,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2611,10 +2700,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>9</v>
@@ -2634,10 +2723,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>9</v>
@@ -2657,10 +2746,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>7</v>
@@ -2680,10 +2769,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>10</v>
@@ -2705,10 +2794,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>9</v>
@@ -2719,10 +2808,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>8</v>
@@ -2733,10 +2822,10 @@
         <v>15</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>6</v>
@@ -2747,10 +2836,10 @@
         <v>75</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>9</v>
@@ -2770,10 +2859,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>9</v>
@@ -2795,10 +2884,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>7</v>
@@ -2809,10 +2898,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>6</v>
@@ -2823,10 +2912,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>6</v>
@@ -2837,10 +2926,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>6</v>
@@ -2851,10 +2940,10 @@
         <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>5</v>
@@ -2865,10 +2954,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>5</v>
@@ -2899,10 +2988,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>9</v>
@@ -2924,10 +3013,10 @@
         <v>24</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>5</v>
@@ -2944,10 +3033,10 @@
         <v>27</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>10</v>
@@ -2967,10 +3056,10 @@
         <v>30</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>10</v>
@@ -2992,10 +3081,10 @@
         <v>30</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>7</v>
@@ -3006,10 +3095,10 @@
         <v>30</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>6</v>
@@ -3020,10 +3109,10 @@
         <v>30</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>6</v>
@@ -3054,10 +3143,10 @@
         <v>36</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>9</v>
@@ -3077,10 +3166,10 @@
         <v>39</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>10</v>
@@ -3100,10 +3189,10 @@
         <v>42</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>7</v>
@@ -3125,10 +3214,10 @@
         <v>42</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>5</v>
@@ -3139,10 +3228,10 @@
         <v>42</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>4</v>
@@ -3159,10 +3248,10 @@
         <v>46</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>9</v>
@@ -3184,10 +3273,10 @@
         <v>46</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>9</v>
@@ -3198,10 +3287,10 @@
         <v>46</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>6</v>
@@ -3212,10 +3301,10 @@
         <v>46</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>5</v>
@@ -3232,10 +3321,10 @@
         <v>49</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>9</v>
@@ -3283,10 +3372,10 @@
         <v>58</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>9</v>
@@ -3306,10 +3395,10 @@
         <v>61</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>8</v>
@@ -3331,10 +3420,10 @@
         <v>61</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>7</v>
@@ -3351,10 +3440,10 @@
         <v>64</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>10</v>
@@ -3374,10 +3463,10 @@
         <v>67</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>10</v>
@@ -3399,10 +3488,10 @@
         <v>67</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>8</v>
@@ -3413,10 +3502,10 @@
         <v>67</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>7</v>
@@ -3427,10 +3516,10 @@
         <v>67</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="F45" s="0" t="n">
         <v>5</v>
@@ -3458,13 +3547,13 @@
         <v>73</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>10</v>
@@ -3519,10 +3608,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3549,6 +3638,9 @@
       <c r="F1" s="2" t="n">
         <v>45782</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -3560,6 +3652,10 @@
       <c r="F2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">SUM(B2:F2)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -3573,6 +3669,10 @@
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">SUM(B3:F3)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3585,6 +3685,10 @@
       <c r="F4" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">SUM(B4:F4)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -3602,6 +3706,10 @@
       <c r="F5" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">SUM(B5:F5)</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -3616,6 +3724,10 @@
       <c r="F6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">SUM(B6:F6)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -3627,6 +3739,10 @@
       <c r="F7" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <f aca="false">SUM(B7:F7)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -3641,6 +3757,10 @@
       <c r="E8" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">SUM(B8:F8)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -3658,6 +3778,10 @@
       <c r="F9" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">SUM(B9:F9)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -3672,6 +3796,10 @@
       <c r="F10" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">SUM(B10:F10)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -3680,6 +3808,10 @@
       <c r="F11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">SUM(B11:F11)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -3697,6 +3829,10 @@
       <c r="F12" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <f aca="false">SUM(B12:F12)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -3714,6 +3850,10 @@
       <c r="F13" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">SUM(B13:F13)</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -3725,6 +3865,10 @@
       <c r="D14" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">SUM(B14:F14)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -3739,6 +3883,10 @@
       <c r="F15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">SUM(B15:F15)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -3750,11 +3898,19 @@
       <c r="F16" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">SUM(B16:F16)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">SUM(B17:F17)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -3769,6 +3925,10 @@
       <c r="F18" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">SUM(B18:F18)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -3780,6 +3940,10 @@
       <c r="F19" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">SUM(B19:F19)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
@@ -3794,6 +3958,10 @@
       <c r="F20" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">SUM(B20:F20)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
@@ -3805,6 +3973,10 @@
       <c r="F21" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">SUM(B21:F21)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
@@ -3819,6 +3991,10 @@
       <c r="F22" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">SUM(B22:F22)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -3830,6 +4006,10 @@
       <c r="F23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">SUM(B23:F23)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -3841,15 +4021,27 @@
       <c r="F24" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">SUM(B24:F24)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>75</v>
       </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">SUM(B25:F25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>77</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">SUM(B26:F26)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3868,10 +4060,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P23" activeCellId="0" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3918,13 +4110,19 @@
         <v>85</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>87</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -3958,8 +4156,23 @@
       <c r="L2" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <f aca="false">L2+M2/2</f>
+        <v>12</v>
+      </c>
+      <c r="O2" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C2,E2,G2,I2,J2,N2),0)</f>
+        <v>9</v>
+      </c>
+      <c r="P2" s="0" t="str">
+        <f aca="false">IF(O2&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -3984,8 +4197,23 @@
       <c r="L3" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <f aca="false">L3+M3/2</f>
+        <v>13</v>
+      </c>
+      <c r="O3" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C3,E3,G3,I3,J3,N3),0)</f>
+        <v>9</v>
+      </c>
+      <c r="P3" s="0" t="str">
+        <f aca="false">IF(O3&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -4013,8 +4241,23 @@
       <c r="L4" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <f aca="false">L4+M4/2</f>
+        <v>11</v>
+      </c>
+      <c r="O4" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C4,E4,G4,I4,J4,N4),0)</f>
+        <v>9</v>
+      </c>
+      <c r="P4" s="0" t="str">
+        <f aca="false">IF(O4&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>5</v>
       </c>
@@ -4040,8 +4283,23 @@
       <c r="L5" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <f aca="false">L5+M5/2</f>
+        <v>17.5</v>
+      </c>
+      <c r="O5" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C5,E5,G5,I5,J5,N5),0)</f>
+        <v>10</v>
+      </c>
+      <c r="P5" s="0" t="str">
+        <f aca="false">IF(O5&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>6</v>
       </c>
@@ -4066,8 +4324,23 @@
       <c r="L6" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <f aca="false">L6+M6/2</f>
+        <v>12</v>
+      </c>
+      <c r="O6" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C6,E6,G6,I6,J6,N6),0)</f>
+        <v>8</v>
+      </c>
+      <c r="P6" s="0" t="str">
+        <f aca="false">IF(O6&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>7</v>
       </c>
@@ -4093,8 +4366,23 @@
       <c r="L7" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <f aca="false">L7+M7/2</f>
+        <v>9</v>
+      </c>
+      <c r="O7" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C7,E7,G7,I7,J7,N7),0)</f>
+        <v>8</v>
+      </c>
+      <c r="P7" s="0" t="str">
+        <f aca="false">IF(O7&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>8</v>
       </c>
@@ -4119,8 +4407,23 @@
       <c r="L8" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <f aca="false">L8+M8/2</f>
+        <v>7</v>
+      </c>
+      <c r="O8" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C8,E8,G8,I8,J8,N8),0)</f>
+        <v>8</v>
+      </c>
+      <c r="P8" s="0" t="str">
+        <f aca="false">IF(O8&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>9</v>
       </c>
@@ -4146,8 +4449,23 @@
       <c r="L9" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <f aca="false">L9+M9/2</f>
+        <v>14</v>
+      </c>
+      <c r="O9" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C9,E9,G9,I9,J9,N9),0)</f>
+        <v>10</v>
+      </c>
+      <c r="P9" s="0" t="str">
+        <f aca="false">IF(O9&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>10</v>
       </c>
@@ -4175,8 +4493,23 @@
       <c r="L10" s="0" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">L10+M10/2</f>
+        <v>14</v>
+      </c>
+      <c r="O10" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C10,E10,G10,I10,J10,N10),0)</f>
+        <v>9</v>
+      </c>
+      <c r="P10" s="0" t="str">
+        <f aca="false">IF(O10&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>11</v>
       </c>
@@ -4207,8 +4540,23 @@
       <c r="L11" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <f aca="false">L11+M11/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="O11" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C11,E11,G11,I11,J11,N11),0)</f>
+        <v>4</v>
+      </c>
+      <c r="P11" s="0" t="str">
+        <f aca="false">IF(O11&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>12</v>
       </c>
@@ -4233,8 +4581,23 @@
       <c r="L12" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <f aca="false">L12+M12/2</f>
+        <v>8</v>
+      </c>
+      <c r="O12" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C12,E12,G12,I12,J12,N12),0)</f>
+        <v>8</v>
+      </c>
+      <c r="P12" s="0" t="str">
+        <f aca="false">IF(O12&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>14</v>
       </c>
@@ -4259,8 +4622,23 @@
       <c r="L13" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <f aca="false">L13+M13/2</f>
+        <v>15.5</v>
+      </c>
+      <c r="O13" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C13,E13,G13,I13,J13,N13),0)</f>
+        <v>10</v>
+      </c>
+      <c r="P13" s="0" t="str">
+        <f aca="false">IF(O13&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>15</v>
       </c>
@@ -4285,8 +4663,23 @@
       <c r="L14" s="0" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">L14+M14/2</f>
+        <v>12.5</v>
+      </c>
+      <c r="O14" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C14,E14,G14,I14,J14,N14),0)</f>
+        <v>6</v>
+      </c>
+      <c r="P14" s="0" t="str">
+        <f aca="false">IF(O14&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>16</v>
       </c>
@@ -4311,8 +4704,23 @@
       <c r="L15" s="0" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">L15+M15/2</f>
+        <v>9</v>
+      </c>
+      <c r="O15" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C15,E15,G15,I15,J15,N15),0)</f>
+        <v>7</v>
+      </c>
+      <c r="P15" s="0" t="str">
+        <f aca="false">IF(O15&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>17</v>
       </c>
@@ -4337,8 +4745,23 @@
       <c r="L16" s="0" t="n">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">L16+M16/2</f>
+        <v>10</v>
+      </c>
+      <c r="O16" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C16,E16,G16,I16,J16,N16),0)</f>
+        <v>9</v>
+      </c>
+      <c r="P16" s="0" t="str">
+        <f aca="false">IF(O16&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>18</v>
       </c>
@@ -4363,8 +4786,23 @@
       <c r="L17" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <f aca="false">L17+M17/2</f>
+        <v>9</v>
+      </c>
+      <c r="O17" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C17,E17,G17,I17,J17,N17),0)</f>
+        <v>5</v>
+      </c>
+      <c r="P17" s="0" t="str">
+        <f aca="false">IF(O17&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>19</v>
       </c>
@@ -4395,8 +4833,23 @@
       <c r="L18" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <f aca="false">L18+M18/2</f>
+        <v>5</v>
+      </c>
+      <c r="O18" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C18,E18,G18,I18,J18,N18),0)</f>
+        <v>7</v>
+      </c>
+      <c r="P18" s="0" t="str">
+        <f aca="false">IF(O18&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>20</v>
       </c>
@@ -4421,8 +4874,23 @@
       <c r="L19" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <f aca="false">L19+M19/2</f>
+        <v>2</v>
+      </c>
+      <c r="O19" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C19,E19,G19,I19,J19,N19),0)</f>
+        <v>5</v>
+      </c>
+      <c r="P19" s="0" t="str">
+        <f aca="false">IF(O19&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>21</v>
       </c>
@@ -4453,8 +4921,23 @@
       <c r="L20" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <f aca="false">L20+M20/2</f>
+        <v>13.5</v>
+      </c>
+      <c r="O20" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C20,E20,G20,I20,J20,N20),0)</f>
+        <v>8</v>
+      </c>
+      <c r="P20" s="0" t="str">
+        <f aca="false">IF(O20&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>22</v>
       </c>
@@ -4482,8 +4965,23 @@
       <c r="L21" s="0" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <f aca="false">L21+M21/2</f>
+        <v>13</v>
+      </c>
+      <c r="O21" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C21,E21,G21,I21,J21,N21),0)</f>
+        <v>9</v>
+      </c>
+      <c r="P21" s="0" t="str">
+        <f aca="false">IF(O21&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>23</v>
       </c>
@@ -4508,8 +5006,23 @@
       <c r="L22" s="0" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M22" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <f aca="false">L22+M22/2</f>
+        <v>14</v>
+      </c>
+      <c r="O22" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C22,E22,G22,I22,J22,N22),0)</f>
+        <v>10</v>
+      </c>
+      <c r="P22" s="0" t="str">
+        <f aca="false">IF(O22&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>24</v>
       </c>
@@ -4539,6 +5052,21 @@
       </c>
       <c r="L23" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <f aca="false">L23+M23/2</f>
+        <v>9.5</v>
+      </c>
+      <c r="O23" s="4" t="n">
+        <f aca="false">ROUND(AVERAGE(C23,E23,G23,I23,J23,N23),0)</f>
+        <v>7</v>
+      </c>
+      <c r="P23" s="0" t="str">
+        <f aca="false">IF(O23&lt;7,"TEP","TEA")</f>
+        <v>TEA</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4551,6 +5079,21 @@
       <c r="L24" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="M24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <f aca="false">L24+M24/2</f>
+        <v>2</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(C24,E24,G24,I24,J24,N24),0)</f>
+        <v>2</v>
+      </c>
+      <c r="P24" s="0" t="str">
+        <f aca="false">IF(O24&lt;7,"TEP","TEA")</f>
+        <v>TEP</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -4562,6 +5105,17 @@
       <c r="L25" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="M25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <f aca="false">L25+M25/2</f>
+        <v>10</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(C25,E25,G25,I25,J25,N25),0)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -4570,8 +5124,29 @@
       <c r="B26" s="0" t="s">
         <v>77</v>
       </c>
+      <c r="M26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <f aca="false">L26+M26/2</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <f aca="false">ROUND(AVERAGE(C26,E26,G26,I26,J26,N26),0)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="O2:O23">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P24">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"TEP"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4589,7 +5164,7 @@
   </sheetPr>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4600,19 +5175,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5644,7 +6219,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5658,22 +6233,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5687,10 +6262,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>10</v>
@@ -5710,10 +6285,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>9</v>
@@ -5735,10 +6310,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>8</v>
@@ -5749,10 +6324,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>7</v>
@@ -5763,10 +6338,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>2</v>
@@ -5783,10 +6358,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>10</v>
@@ -5808,10 +6383,10 @@
         <v>12</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>10</v>
@@ -5822,10 +6397,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
@@ -5836,10 +6411,10 @@
         <v>12</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>2</v>
@@ -5850,10 +6425,10 @@
         <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>2</v>
@@ -5864,10 +6439,10 @@
         <v>12</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>1</v>
@@ -5884,10 +6459,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>7</v>
@@ -5907,10 +6482,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>1</v>
@@ -5944,10 +6519,10 @@
         <v>24</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>8</v>
@@ -5969,10 +6544,10 @@
         <v>24</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>8</v>
@@ -5983,10 +6558,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>8</v>
@@ -5997,10 +6572,10 @@
         <v>24</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>8</v>
@@ -6011,10 +6586,10 @@
         <v>24</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>8</v>
@@ -6025,10 +6600,10 @@
         <v>24</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>5</v>
@@ -6039,10 +6614,10 @@
         <v>24</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>4</v>
@@ -6053,10 +6628,10 @@
         <v>24</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>3</v>
@@ -6073,10 +6648,10 @@
         <v>27</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>10</v>
@@ -6098,10 +6673,10 @@
         <v>27</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>9</v>
@@ -6132,10 +6707,10 @@
         <v>33</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>1</v>
@@ -6155,10 +6730,10 @@
         <v>36</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>10</v>
@@ -6178,10 +6753,10 @@
         <v>39</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>10</v>
@@ -6203,10 +6778,10 @@
         <v>39</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>8</v>
@@ -6217,10 +6792,10 @@
         <v>39</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>3</v>
@@ -6251,10 +6826,10 @@
         <v>46</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>5</v>
@@ -6276,10 +6851,10 @@
         <v>46</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>4</v>
@@ -6290,10 +6865,10 @@
         <v>46</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>4</v>
@@ -6304,10 +6879,10 @@
         <v>46</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>3</v>
@@ -6318,10 +6893,10 @@
         <v>46</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>3</v>
@@ -6332,10 +6907,10 @@
         <v>46</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>3</v>
@@ -6352,10 +6927,10 @@
         <v>49</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>8</v>
@@ -6377,10 +6952,10 @@
         <v>49</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>7</v>
@@ -6391,10 +6966,10 @@
         <v>49</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>7</v>
@@ -6405,10 +6980,10 @@
         <v>49</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>6</v>
@@ -6419,10 +6994,10 @@
         <v>49</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>5</v>
@@ -6433,10 +7008,10 @@
         <v>49</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>0</v>
@@ -6495,10 +7070,10 @@
         <v>61</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>10</v>
@@ -6520,10 +7095,10 @@
         <v>61</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>9</v>
@@ -6540,10 +7115,10 @@
         <v>64</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>10</v>
@@ -6565,10 +7140,10 @@
         <v>64</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>9</v>
@@ -6579,10 +7154,10 @@
         <v>64</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>8</v>
@@ -6593,10 +7168,10 @@
         <v>64</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>4</v>
@@ -6607,10 +7182,10 @@
         <v>64</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>1</v>
@@ -6627,10 +7202,10 @@
         <v>67</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>10</v>
@@ -6652,10 +7227,10 @@
         <v>67</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>9</v>
@@ -6666,10 +7241,10 @@
         <v>67</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>8</v>
@@ -6680,10 +7255,10 @@
         <v>67</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F58" s="0" t="n">
         <v>6</v>
@@ -6694,10 +7269,10 @@
         <v>67</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F59" s="0" t="n">
         <v>3</v>
@@ -6765,7 +7340,7 @@
   </sheetPr>
   <dimension ref="C1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -6780,19 +7355,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="H1" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6800,7 +7375,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>8</v>
@@ -6814,7 +7389,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>8</v>
@@ -6828,7 +7403,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>8</v>
@@ -6850,7 +7425,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>4</v>
@@ -6861,7 +7436,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>4</v>
@@ -6872,7 +7447,7 @@
         <v>70</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>4</v>
@@ -6883,7 +7458,7 @@
         <v>70</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>3</v>
@@ -6894,7 +7469,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3</v>
@@ -6905,7 +7480,7 @@
         <v>70</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2</v>
@@ -6929,7 +7504,7 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -6946,22 +7521,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6989,10 +7564,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>8</v>
@@ -7014,10 +7589,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>7</v>
@@ -7028,10 +7603,10 @@
         <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>6</v>
@@ -7042,10 +7617,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>6</v>
@@ -7056,10 +7631,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>4</v>
@@ -7076,10 +7651,10 @@
         <v>12</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>8</v>
@@ -7101,10 +7676,10 @@
         <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>6</v>
@@ -7115,10 +7690,10 @@
         <v>12</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
@@ -7135,10 +7710,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>8</v>
@@ -7158,10 +7733,10 @@
         <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>8</v>
@@ -7183,10 +7758,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>8</v>
@@ -7203,10 +7778,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>10</v>
@@ -7228,10 +7803,10 @@
         <v>21</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>9</v>
@@ -7242,10 +7817,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>2</v>
@@ -7256,10 +7831,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>1</v>
@@ -7276,10 +7851,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>8</v>
@@ -7299,10 +7874,10 @@
         <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>9</v>
@@ -7322,10 +7897,10 @@
         <v>30</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>6</v>
@@ -7345,10 +7920,10 @@
         <v>33</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>8</v>
@@ -7368,10 +7943,10 @@
         <v>36</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>9</v>
@@ -7391,10 +7966,10 @@
         <v>39</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>9</v>
@@ -7414,10 +7989,10 @@
         <v>42</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>6</v>
@@ -7437,10 +8012,10 @@
         <v>46</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>8</v>
@@ -7462,10 +8037,10 @@
         <v>46</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>8</v>
@@ -7476,10 +8051,10 @@
         <v>46</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>7</v>
@@ -7490,10 +8065,10 @@
         <v>46</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>7</v>
@@ -7510,10 +8085,10 @@
         <v>49</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>10</v>
@@ -7535,10 +8110,10 @@
         <v>49</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>8</v>
@@ -7549,10 +8124,10 @@
         <v>49</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>8</v>
@@ -7563,10 +8138,10 @@
         <v>49</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F32" s="0" t="n">
         <v>6</v>
@@ -7583,10 +8158,10 @@
         <v>52</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>8</v>
@@ -7608,10 +8183,10 @@
         <v>52</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>4</v>
@@ -7628,10 +8203,10 @@
         <v>55</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>9</v>
@@ -7653,10 +8228,10 @@
         <v>55</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="F36" s="0" t="n">
         <v>8</v>
@@ -7667,10 +8242,10 @@
         <v>55</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F37" s="0" t="n">
         <v>2</v>
@@ -7687,10 +8262,10 @@
         <v>58</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>9</v>
@@ -7712,10 +8287,10 @@
         <v>58</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>8</v>
@@ -7726,10 +8301,10 @@
         <v>58</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>7</v>
@@ -7740,10 +8315,10 @@
         <v>58</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="F41" s="0" t="n">
         <v>6</v>
@@ -7754,10 +8329,10 @@
         <v>58</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F42" s="0" t="n">
         <v>6</v>
@@ -7768,10 +8343,10 @@
         <v>58</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="F43" s="0" t="n">
         <v>5</v>
@@ -7782,10 +8357,10 @@
         <v>58</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="F44" s="0" t="n">
         <v>2</v>
@@ -7816,10 +8391,10 @@
         <v>64</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F46" s="0" t="n">
         <v>7</v>
@@ -7839,10 +8414,10 @@
         <v>67</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F47" s="0" t="n">
         <v>8</v>
@@ -7862,10 +8437,10 @@
         <v>70</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="F48" s="0" t="n">
         <v>5</v>
@@ -7917,7 +8492,7 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -7933,22 +8508,22 @@
         <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="G1" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7956,10 +8531,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>6</v>
@@ -7981,10 +8556,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>6</v>
@@ -7995,10 +8570,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>5</v>
@@ -8009,10 +8584,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -8023,10 +8598,10 @@
         <v>61</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>8</v>
@@ -8048,10 +8623,10 @@
         <v>61</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>5</v>
@@ -8062,10 +8637,10 @@
         <v>61</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>5</v>
@@ -8076,10 +8651,10 @@
         <v>61</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>4</v>
@@ -8090,10 +8665,10 @@
         <v>61</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
@@ -8104,10 +8679,10 @@
         <v>61</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3</v>
@@ -8118,10 +8693,10 @@
         <v>61</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>2</v>
@@ -8132,10 +8707,10 @@
         <v>61</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>2</v>
@@ -8146,10 +8721,10 @@
         <v>70</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>7</v>
@@ -8171,10 +8746,10 @@
         <v>70</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>6</v>
@@ -8185,10 +8760,10 @@
         <v>70</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>5</v>
@@ -8199,10 +8774,10 @@
         <v>70</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>5</v>
@@ -8213,10 +8788,10 @@
         <v>70</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>5</v>
@@ -8227,10 +8802,10 @@
         <v>70</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>3</v>
@@ -8254,7 +8829,7 @@
   </sheetPr>
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -8271,22 +8846,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8300,10 +8875,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>9.5</v>
@@ -8323,10 +8898,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>8.33</v>
@@ -8346,10 +8921,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>10</v>
@@ -8369,10 +8944,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>9.5</v>
@@ -8392,10 +8967,10 @@
         <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>10</v>
@@ -8415,10 +8990,10 @@
         <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>10</v>
@@ -8438,10 +9013,10 @@
         <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>10</v>
@@ -8461,10 +9036,10 @@
         <v>27</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>10</v>
@@ -8484,10 +9059,10 @@
         <v>30</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>9.5</v>
@@ -8521,10 +9096,10 @@
         <v>36</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>10</v>
@@ -8544,10 +9119,10 @@
         <v>39</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>10</v>
@@ -8567,10 +9142,10 @@
         <v>42</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>9.33</v>
@@ -8590,10 +9165,10 @@
         <v>46</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>9.33</v>
@@ -8613,10 +9188,10 @@
         <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>9.33</v>
@@ -8636,10 +9211,10 @@
         <v>52</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>10</v>
@@ -8659,10 +9234,10 @@
         <v>55</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>9.42</v>
@@ -8682,10 +9257,10 @@
         <v>58</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>9.33</v>
@@ -8707,10 +9282,10 @@
         <v>58</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>8.33</v>
@@ -8721,10 +9296,10 @@
         <v>58</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>3</v>
@@ -8741,10 +9316,10 @@
         <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>9.42</v>
@@ -8764,10 +9339,10 @@
         <v>64</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>10</v>
@@ -8787,10 +9362,10 @@
         <v>67</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>10</v>
@@ -8810,10 +9385,10 @@
         <v>70</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>10</v>
@@ -8870,7 +9445,7 @@
   </sheetPr>
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -8887,22 +9462,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8930,10 +9505,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>8</v>
@@ -8953,10 +9528,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>8</v>
@@ -8976,10 +9551,10 @@
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>10</v>
@@ -9001,10 +9576,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>7</v>
@@ -9021,10 +9596,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>8</v>
@@ -9044,10 +9619,10 @@
         <v>21</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>10</v>
@@ -9069,10 +9644,10 @@
         <v>21</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>9</v>
@@ -9083,10 +9658,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
@@ -9097,10 +9672,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>6</v>
@@ -9111,10 +9686,10 @@
         <v>21</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>6</v>
@@ -9125,10 +9700,10 @@
         <v>21</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>5</v>
@@ -9145,10 +9720,10 @@
         <v>24</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>10</v>
@@ -9168,10 +9743,10 @@
         <v>27</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>10</v>
@@ -9193,10 +9768,10 @@
         <v>27</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>10</v>
@@ -9207,10 +9782,10 @@
         <v>27</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>10</v>
@@ -9221,10 +9796,10 @@
         <v>27</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>10</v>
@@ -9235,10 +9810,10 @@
         <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F19" s="0" t="n">
         <v>9</v>
@@ -9249,10 +9824,10 @@
         <v>27</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>9</v>
@@ -9263,10 +9838,10 @@
         <v>27</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>4</v>
@@ -9283,10 +9858,10 @@
         <v>30</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>8</v>
@@ -9306,10 +9881,10 @@
         <v>33</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>3</v>
@@ -9343,10 +9918,10 @@
         <v>39</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>10</v>
@@ -9380,10 +9955,10 @@
         <v>46</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>5</v>
@@ -9403,10 +9978,10 @@
         <v>49</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F28" s="0" t="n">
         <v>10</v>
@@ -9454,10 +10029,10 @@
         <v>58</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="F31" s="0" t="n">
         <v>9</v>
@@ -9505,10 +10080,10 @@
         <v>67</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>8</v>
@@ -9528,10 +10103,10 @@
         <v>70</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
agregados de archivos intermedio y cerrar notas
</commit_message>
<xml_diff>
--- a/inasistencias-5a-InstrumentalYsistElect/alumnos-5a-InstrumentalYsistElect.xlsx
+++ b/inasistencias-5a-InstrumentalYsistElect/alumnos-5a-InstrumentalYsistElect.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="633">
   <si>
     <t xml:space="preserve">nro</t>
   </si>
@@ -1952,7 +1952,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1975,14 +1975,8 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1998,7 +1992,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9800"/>
-        <bgColor rgb="FFFF6600"/>
+        <bgColor rgb="FFFFC107"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC107"/>
+        <bgColor rgb="FFFF9800"/>
       </patternFill>
     </fill>
   </fills>
@@ -2036,7 +2036,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2057,23 +2057,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2086,50 +2082,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF232629"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF9800"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCC0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -2220,7 +2173,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFC107"/>
       <rgbColor rgb="FFFF9800"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -2245,16 +2198,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.2"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="15" min="5" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.33"/>
@@ -2669,11 +2621,11 @@
       <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>12</v>
+      <c r="E8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>45848</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>12</v>
@@ -2701,15 +2653,15 @@
       </c>
       <c r="O8" s="0" t="n">
         <f aca="false">COUNTIF(E8:N8,"P")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P8" s="0" t="n">
         <f aca="false">O8</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="AB8" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(AA8,Y8,X8,W8,U8,S8,P8),0)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,6 +2876,9 @@
         <f aca="false">O12</f>
         <v>10</v>
       </c>
+      <c r="S12" s="5" t="n">
+        <v>10</v>
+      </c>
       <c r="AB12" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(AA12,Y12,X12,W12,U12,S12,P12),0)</f>
         <v>10</v>
@@ -3181,8 +3136,8 @@
       <c r="I17" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="0" t="s">
-        <v>28</v>
+      <c r="J17" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="K17" s="0" t="s">
         <v>12</v>
@@ -3198,15 +3153,18 @@
       </c>
       <c r="O17" s="0" t="n">
         <f aca="false">COUNTIF(E17:N17,"P")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P17" s="0" t="n">
         <f aca="false">O17</f>
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AA17" s="0" t="n">
+        <v>10</v>
       </c>
       <c r="AB17" s="0" t="n">
         <f aca="false">ROUND(AVERAGE(AA17,Y17,X17,W17,U17,S17,P17),0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3712,11 +3670,11 @@
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E27" s="0" t="n">
         <f aca="false">COUNTIF(E2:E23,"P")</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" s="0" t="n">
         <f aca="false">COUNTIF(F2:F23,"P")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G27" s="0" t="n">
         <f aca="false">COUNTIF(G2:G23,"P")</f>
@@ -3732,7 +3690,7 @@
       </c>
       <c r="J27" s="0" t="n">
         <f aca="false">COUNTIF(J2:J26,"P")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K27" s="0" t="n">
         <f aca="false">COUNTIF(K2:K26,"P")</f>
@@ -3769,11 +3727,11 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.58"/>
@@ -3854,11 +3812,11 @@
   </sheetPr>
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
@@ -4464,11 +4422,11 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
   </cols>
@@ -4547,11 +4505,11 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.04"/>
@@ -5259,11 +5217,11 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.07"/>
@@ -5345,11 +5303,11 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -5743,11 +5701,11 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.16"/>
@@ -5829,11 +5787,11 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.2"/>
   </cols>
@@ -6296,11 +6254,11 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I47" activeCellId="0" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.2"/>
@@ -7244,11 +7202,11 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.2"/>
@@ -7951,15 +7909,15 @@
   </sheetPr>
   <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC22" activeCellId="0" sqref="AC22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA17" activeCellId="0" sqref="AA17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.2"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="15" min="3" style="0" width="9.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="0" width="9.39"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="0" width="11.19"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.57"/>
@@ -8032,7 +7990,7 @@
       <c r="U1" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="W1" s="0" t="s">
@@ -8095,11 +8053,11 @@
         <f aca="false">L2+N2/2</f>
         <v>12</v>
       </c>
-      <c r="P2" s="6" t="n">
+      <c r="P2" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C2,E2,G2,I2,J2,O2),0)</f>
         <v>9</v>
       </c>
-      <c r="Q2" s="0" t="str">
+      <c r="Q2" s="8" t="str">
         <f aca="false">IF(P2&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8121,7 +8079,7 @@
       <c r="AA2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB2" s="7" t="n">
+      <c r="AB2" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA2,Y2,X2,W2,U2,S2,P2),0)</f>
         <v>8</v>
       </c>
@@ -8158,11 +8116,11 @@
         <f aca="false">L3+N3/2</f>
         <v>13</v>
       </c>
-      <c r="P3" s="6" t="n">
+      <c r="P3" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C3,E3,G3,I3,J3,O3),0)</f>
         <v>9</v>
       </c>
-      <c r="Q3" s="0" t="str">
+      <c r="Q3" s="8" t="str">
         <f aca="false">IF(P3&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8184,7 +8142,7 @@
       <c r="AA3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB3" s="7" t="n">
+      <c r="AB3" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA3,Y3,X3,W3,U3,S3,P3),0)</f>
         <v>8</v>
       </c>
@@ -8224,11 +8182,11 @@
         <f aca="false">L4+N4/2</f>
         <v>13</v>
       </c>
-      <c r="P4" s="6" t="n">
+      <c r="P4" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C4,E4,G4,I4,J4,O4),0)</f>
         <v>9</v>
       </c>
-      <c r="Q4" s="0" t="str">
+      <c r="Q4" s="8" t="str">
         <f aca="false">IF(P4&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8250,7 +8208,7 @@
       <c r="AA4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB4" s="7" t="n">
+      <c r="AB4" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA4,Y4,X4,W4,U4,S4,P4),0)</f>
         <v>9</v>
       </c>
@@ -8288,11 +8246,11 @@
         <f aca="false">L5+N5/2</f>
         <v>17.5</v>
       </c>
-      <c r="P5" s="6" t="n">
+      <c r="P5" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C5,E5,G5,I5,J5,O5),0)</f>
         <v>10</v>
       </c>
-      <c r="Q5" s="0" t="str">
+      <c r="Q5" s="8" t="str">
         <f aca="false">IF(P5&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8314,7 +8272,7 @@
       <c r="AA5" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB5" s="7" t="n">
+      <c r="AB5" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA5,Y5,X5,W5,U5,S5,P5),0)</f>
         <v>9</v>
       </c>
@@ -8351,18 +8309,18 @@
         <f aca="false">L6+N6/2</f>
         <v>1</v>
       </c>
-      <c r="P6" s="6" t="n">
+      <c r="P6" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C6,E6,G6,I6,J6,O6),0)</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="0" t="str">
+      <c r="Q6" s="8" t="str">
         <f aca="false">IF(P6&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
-      <c r="S6" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="T6" s="9" t="n">
+      <c r="S6" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="T6" s="6" t="n">
         <v>45848</v>
       </c>
       <c r="U6" s="0" t="n">
@@ -8380,7 +8338,7 @@
       <c r="AA6" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB6" s="7" t="n">
+      <c r="AB6" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA6,Y6,X6,W6,U6,S6,P6),0)</f>
         <v>6</v>
       </c>
@@ -8420,11 +8378,11 @@
         <f aca="false">L7+N7/2</f>
         <v>12</v>
       </c>
-      <c r="P7" s="6" t="n">
+      <c r="P7" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C7,E7,G7,I7,J7,O7),0)</f>
         <v>8</v>
       </c>
-      <c r="Q7" s="0" t="str">
+      <c r="Q7" s="8" t="str">
         <f aca="false">IF(P7&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8446,7 +8404,7 @@
       <c r="AA7" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="AB7" s="7" t="n">
+      <c r="AB7" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA7,Y7,X7,W7,U7,S7,P7),0)</f>
         <v>7</v>
       </c>
@@ -8461,8 +8419,11 @@
       <c r="C8" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <v>1</v>
+      <c r="E8" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>45848</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>9</v>
@@ -8477,7 +8438,7 @@
       <c r="L8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="M8" s="9" t="n">
+      <c r="M8" s="6" t="n">
         <v>45818</v>
       </c>
       <c r="N8" s="0" t="n">
@@ -8487,24 +8448,24 @@
         <f aca="false">L8+N8/2</f>
         <v>9</v>
       </c>
-      <c r="P8" s="6" t="n">
+      <c r="P8" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C8,E8,G8,I8,J8,O8),0)</f>
-        <v>8</v>
-      </c>
-      <c r="Q8" s="0" t="str">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="8" t="str">
         <f aca="false">IF(P8&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
-      <c r="S8" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="T8" s="9" t="n">
+      <c r="S8" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="T8" s="6" t="n">
         <v>45846</v>
       </c>
-      <c r="U8" s="8" t="n">
+      <c r="U8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="V8" s="9" t="n">
+      <c r="V8" s="6" t="n">
         <v>45849</v>
       </c>
       <c r="W8" s="0" t="n">
@@ -8519,9 +8480,9 @@
       <c r="AA8" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB8" s="7" t="n">
+      <c r="AB8" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA8,Y8,X8,W8,U8,S8,P8),0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8556,11 +8517,11 @@
         <f aca="false">L9+N9/2</f>
         <v>7</v>
       </c>
-      <c r="P9" s="6" t="n">
+      <c r="P9" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C9,E9,G9,I9,J9,O9),0)</f>
         <v>8</v>
       </c>
-      <c r="Q9" s="0" t="str">
+      <c r="Q9" s="8" t="str">
         <f aca="false">IF(P9&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8576,16 +8537,16 @@
       <c r="X9" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="Y9" s="8" t="n">
-        <v>9</v>
-      </c>
-      <c r="Z9" s="9" t="n">
+      <c r="Y9" s="5" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z9" s="6" t="n">
         <v>45852</v>
       </c>
       <c r="AA9" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB9" s="7" t="n">
+      <c r="AB9" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA9,Y9,X9,W9,U9,S9,P9),0)</f>
         <v>8</v>
       </c>
@@ -8622,11 +8583,11 @@
         <f aca="false">L10+N10/2</f>
         <v>10</v>
       </c>
-      <c r="P10" s="6" t="n">
+      <c r="P10" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C10,E10,G10,I10,J10,O10),0)</f>
         <v>9</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="8" t="s">
         <v>102</v>
       </c>
       <c r="R10" s="0" t="s">
@@ -8650,7 +8611,7 @@
       <c r="AA10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AB10" s="7" t="n">
+      <c r="AB10" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA10,Y10,X10,W10,U10,S10,P10),0)</f>
         <v>3</v>
       </c>
@@ -8691,11 +8652,11 @@
         <f aca="false">L11+N11/2</f>
         <v>14</v>
       </c>
-      <c r="P11" s="6" t="n">
+      <c r="P11" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C11,E11,G11,I11,J11,O11),0)</f>
         <v>10</v>
       </c>
-      <c r="Q11" s="0" t="str">
+      <c r="Q11" s="8" t="str">
         <f aca="false">IF(P11&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8717,7 +8678,7 @@
       <c r="AA11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB11" s="7" t="n">
+      <c r="AB11" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA11,Y11,X11,W11,U11,S11,P11),0)</f>
         <v>10</v>
       </c>
@@ -8757,16 +8718,16 @@
         <f aca="false">L12+N12/2</f>
         <v>15.5</v>
       </c>
-      <c r="P12" s="6" t="n">
+      <c r="P12" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C12,E12,G12,I12,J12,O12),0)</f>
         <v>9</v>
       </c>
-      <c r="Q12" s="0" t="str">
+      <c r="Q12" s="8" t="str">
         <f aca="false">IF(P12&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
-      <c r="S12" s="0" t="n">
-        <v>1</v>
+      <c r="S12" s="5" t="n">
+        <v>10</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>7</v>
@@ -8783,9 +8744,9 @@
       <c r="AA12" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB12" s="7" t="n">
+      <c r="AB12" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA12,Y12,X12,W12,U12,S12,P12),0)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8826,11 +8787,11 @@
         <f aca="false">L13+N13/2</f>
         <v>7.5</v>
       </c>
-      <c r="P13" s="6" t="n">
+      <c r="P13" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C13,E13,G13,I13,J13,O13),0)</f>
         <v>4</v>
       </c>
-      <c r="Q13" s="0" t="str">
+      <c r="Q13" s="8" t="str">
         <f aca="false">IF(P13&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -8852,7 +8813,7 @@
       <c r="AA13" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB13" s="7" t="n">
+      <c r="AB13" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA13,Y13,X13,W13,U13,S13,P13),0)</f>
         <v>6</v>
       </c>
@@ -8889,11 +8850,11 @@
         <f aca="false">L14+N14/2</f>
         <v>8</v>
       </c>
-      <c r="P14" s="6" t="n">
+      <c r="P14" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C14,E14,G14,I14,J14,O14),0)</f>
         <v>8</v>
       </c>
-      <c r="Q14" s="0" t="str">
+      <c r="Q14" s="8" t="str">
         <f aca="false">IF(P14&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8915,7 +8876,7 @@
       <c r="AA14" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB14" s="7" t="n">
+      <c r="AB14" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA14,Y14,X14,W14,U14,S14,P14),0)</f>
         <v>8</v>
       </c>
@@ -8952,11 +8913,11 @@
         <f aca="false">L15+N15/2</f>
         <v>15.5</v>
       </c>
-      <c r="P15" s="6" t="n">
+      <c r="P15" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C15,E15,G15,I15,J15,O15),0)</f>
         <v>10</v>
       </c>
-      <c r="Q15" s="0" t="str">
+      <c r="Q15" s="8" t="str">
         <f aca="false">IF(P15&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -8978,7 +8939,7 @@
       <c r="AA15" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB15" s="7" t="n">
+      <c r="AB15" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA15,Y15,X15,W15,U15,S15,P15),0)</f>
         <v>9</v>
       </c>
@@ -9015,11 +8976,11 @@
         <f aca="false">L16+N16/2</f>
         <v>12.5</v>
       </c>
-      <c r="P16" s="6" t="n">
+      <c r="P16" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C16,E16,G16,I16,J16,O16),0)</f>
         <v>6</v>
       </c>
-      <c r="Q16" s="0" t="str">
+      <c r="Q16" s="8" t="str">
         <f aca="false">IF(P16&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -9041,7 +9002,7 @@
       <c r="AA16" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="AB16" s="7" t="n">
+      <c r="AB16" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA16,Y16,X16,W16,U16,S16,P16),0)</f>
         <v>6</v>
       </c>
@@ -9065,8 +9026,8 @@
       <c r="I17" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="J17" s="0" t="n">
-        <v>5</v>
+      <c r="J17" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>5</v>
@@ -9078,11 +9039,11 @@
         <f aca="false">L17+N17/2</f>
         <v>9</v>
       </c>
-      <c r="P17" s="6" t="n">
+      <c r="P17" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C17,E17,G17,I17,J17,O17),0)</f>
         <v>7</v>
       </c>
-      <c r="Q17" s="0" t="str">
+      <c r="Q17" s="8" t="str">
         <f aca="false">IF(P17&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -9102,9 +9063,9 @@
         <v>9</v>
       </c>
       <c r="AA17" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="AB17" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB17" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA17,Y17,X17,W17,U17,S17,P17),0)</f>
         <v>8</v>
       </c>
@@ -9141,11 +9102,11 @@
         <f aca="false">L18+N18/2</f>
         <v>10.5</v>
       </c>
-      <c r="P18" s="6" t="n">
+      <c r="P18" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C18,E18,G18,I18,J18,O18),0)</f>
         <v>9</v>
       </c>
-      <c r="Q18" s="0" t="str">
+      <c r="Q18" s="8" t="str">
         <f aca="false">IF(P18&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -9167,7 +9128,7 @@
       <c r="AA18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB18" s="7" t="n">
+      <c r="AB18" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA18,Y18,X18,W18,U18,S18,P18),0)</f>
         <v>8</v>
       </c>
@@ -9204,11 +9165,11 @@
         <f aca="false">L19+N19/2</f>
         <v>9</v>
       </c>
-      <c r="P19" s="6" t="n">
+      <c r="P19" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C19,E19,G19,I19,J19,O19),0)</f>
         <v>5</v>
       </c>
-      <c r="Q19" s="0" t="str">
+      <c r="Q19" s="8" t="str">
         <f aca="false">IF(P19&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -9230,7 +9191,7 @@
       <c r="AA19" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB19" s="7" t="n">
+      <c r="AB19" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA19,Y19,X19,W19,U19,S19,P19),0)</f>
         <v>7</v>
       </c>
@@ -9273,11 +9234,11 @@
         <f aca="false">L20+N20/2</f>
         <v>5</v>
       </c>
-      <c r="P20" s="6" t="n">
+      <c r="P20" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C20,E20,G20,I20,J20,O20),0)</f>
         <v>7</v>
       </c>
-      <c r="Q20" s="0" t="str">
+      <c r="Q20" s="8" t="str">
         <f aca="false">IF(P20&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -9299,7 +9260,7 @@
       <c r="AA20" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="AB20" s="7" t="n">
+      <c r="AB20" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA20,Y20,X20,W20,U20,S20,P20),0)</f>
         <v>6</v>
       </c>
@@ -9336,11 +9297,11 @@
         <f aca="false">L21+N21/2</f>
         <v>11</v>
       </c>
-      <c r="P21" s="6" t="n">
+      <c r="P21" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C20,E21,G21,I21,J21,O21),0)</f>
         <v>5</v>
       </c>
-      <c r="Q21" s="0" t="str">
+      <c r="Q21" s="8" t="str">
         <f aca="false">IF(P21&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -9362,7 +9323,7 @@
       <c r="AA21" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="AB21" s="7" t="n">
+      <c r="AB21" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA21,Y21,X21,W21,U21,S21,P21),0)</f>
         <v>3</v>
       </c>
@@ -9402,11 +9363,11 @@
         <f aca="false">L22+N22/2</f>
         <v>2</v>
       </c>
-      <c r="P22" s="6" t="n">
+      <c r="P22" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C22,E22,G22,I22,J22,O22),0)</f>
         <v>5</v>
       </c>
-      <c r="Q22" s="0" t="str">
+      <c r="Q22" s="8" t="str">
         <f aca="false">IF(P22&lt;7,"TEP","TEA")</f>
         <v>TEP</v>
       </c>
@@ -9428,7 +9389,7 @@
       <c r="AA22" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="AB22" s="7" t="n">
+      <c r="AB22" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA22,Y22,X22,W22,U22,S22,P22),0)</f>
         <v>6</v>
       </c>
@@ -9471,11 +9432,11 @@
         <f aca="false">L23+N23/2</f>
         <v>13.5</v>
       </c>
-      <c r="P23" s="6" t="n">
+      <c r="P23" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C23,E23,G23,I23,J23,O23),0)</f>
         <v>8</v>
       </c>
-      <c r="Q23" s="0" t="str">
+      <c r="Q23" s="8" t="str">
         <f aca="false">IF(P23&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -9497,7 +9458,7 @@
       <c r="AA23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="AB23" s="7" t="n">
+      <c r="AB23" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA23,Y23,X23,W23,U23,S23,P23),0)</f>
         <v>7</v>
       </c>
@@ -9537,11 +9498,11 @@
         <f aca="false">L24+N24/2</f>
         <v>13</v>
       </c>
-      <c r="P24" s="6" t="n">
+      <c r="P24" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C24,E24,G24,I24,J24,O24),0)</f>
         <v>9</v>
       </c>
-      <c r="Q24" s="0" t="str">
+      <c r="Q24" s="8" t="str">
         <f aca="false">IF(P24&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -9563,7 +9524,7 @@
       <c r="AA24" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB24" s="7" t="n">
+      <c r="AB24" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA24,Y24,X24,W24,U24,S24,P24),0)</f>
         <v>8</v>
       </c>
@@ -9600,11 +9561,11 @@
         <f aca="false">L25+N25/2</f>
         <v>14</v>
       </c>
-      <c r="P25" s="6" t="n">
+      <c r="P25" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C25,E25,G25,I25,J25,O25),0)</f>
         <v>10</v>
       </c>
-      <c r="Q25" s="0" t="str">
+      <c r="Q25" s="8" t="str">
         <f aca="false">IF(P25&lt;7,"TEP","TEA")</f>
         <v>TEA</v>
       </c>
@@ -9626,7 +9587,7 @@
       <c r="AA25" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="AB25" s="7" t="n">
+      <c r="AB25" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA25,Y25,X25,W25,U25,S25,P25),0)</f>
         <v>9</v>
       </c>
@@ -9669,7 +9630,7 @@
         <f aca="false">L26+N26/2</f>
         <v>9.5</v>
       </c>
-      <c r="P26" s="6" t="n">
+      <c r="P26" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(C26,E26,G26,I26,J26,O26),0)</f>
         <v>7</v>
       </c>
@@ -9695,29 +9656,29 @@
       <c r="AA26" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="AB26" s="7" t="n">
+      <c r="AB26" s="8" t="n">
         <f aca="false">ROUND(AVERAGE(AA26,Y26,X26,W26,U26,S26,P26),0)</f>
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="P2:P23">
-    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q25">
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"TEP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P24:P26">
-    <cfRule type="cellIs" priority="4" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="4" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2:AB26">
-    <cfRule type="cellIs" priority="5" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" priority="5" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9738,11 +9699,11 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.98"/>
@@ -11221,11 +11182,11 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
@@ -11771,13 +11732,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="20.07"/>
@@ -12849,13 +12810,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="20.2"/>
@@ -13528,11 +13489,11 @@
   </sheetPr>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="20.2"/>
   </cols>
@@ -14583,11 +14544,11 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.95"/>
@@ -14771,11 +14732,11 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.07"/>
   </cols>
@@ -15886,11 +15847,11 @@
   </sheetPr>
   <dimension ref="C1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
@@ -16050,11 +16011,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.58"/>
@@ -16135,11 +16096,11 @@
   </sheetPr>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
@@ -17122,11 +17083,11 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>

</xml_diff>